<commit_message>
Bug Fixes and also created gui_test.py which makes testing GUI convenient
</commit_message>
<xml_diff>
--- a/Arduino/fluidlevelsensorcalibration.xlsx
+++ b/Arduino/fluidlevelsensorcalibration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrine\OneDrive\Desktop\ComputerBoil2023\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63CB7CDE-C4B9-4D16-92C6-1AC8222AFED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA54AB4-5CAB-4A0F-ADBE-47CFC35F3D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8B53C56B-863B-40F0-A689-5F55A9D423B2}"/>
   </bookViews>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Height</t>
+    <t>Height (in)</t>
   </si>
   <si>
-    <t>Analog</t>
+    <t>Height (cm)</t>
+  </si>
+  <si>
+    <t>Analog Reading</t>
   </si>
 </sst>
 </file>
@@ -120,27 +123,63 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:trendline>
@@ -149,7 +188,7 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -163,7 +202,7 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -177,7 +216,7 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -200,9 +239,8 @@
                   <a:pPr>
                     <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
                         </a:schemeClr>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
@@ -221,7 +259,7 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -312,9 +350,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -322,6 +360,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Height (cm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -330,12 +421,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -346,9 +435,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -370,6 +458,73 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Analog Reading</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -378,12 +533,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -394,9 +547,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -431,17 +583,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -504,62 +667,66 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -568,9 +735,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -589,14 +755,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -605,20 +763,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -627,13 +785,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -645,30 +803,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -684,21 +843,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -717,18 +873,62 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -738,66 +938,14 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
   </cs:gridlineMajor>
   <cs:gridlineMinor>
     <cs:lnRef idx="0"/>
@@ -807,14 +955,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -826,14 +973,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -845,14 +992,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -861,14 +1007,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -876,7 +1021,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -889,11 +1034,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -901,14 +1054,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -920,12 +1073,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -941,7 +1101,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -950,9 +1110,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -968,14 +1127,13 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -984,20 +1142,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1009,12 +1164,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1058,6 +1207,20 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0748A241-1812-4214-989E-B278A380571D}" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0">
+  <autoFilter ref="A1:C8" xr:uid="{0748A241-1812-4214-989E-B278A380571D}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{2DAB21D5-5917-4B5B-A662-E43CC222BEC2}" name="Height (in)"/>
+    <tableColumn id="2" xr3:uid="{6C044E2D-4F59-460D-9778-6DF4D19E1EE3}" name="Height (cm)">
+      <calculatedColumnFormula>A2*2.54</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{5EEBCD47-ADB0-4F0B-B776-A0208BE737F0}" name="Analog Reading"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1360,17 +1523,25 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1518,6 +1689,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>